<commit_message>
Added username and passwrod in input.xls
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B88 Selenium\Day26 06-11-2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B88 Selenium\Workspace\framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E07047-9032-43DB-BCB9-A90B5A1D3B3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E481B1B-3118-4C1B-AF9C-B1D753ED5F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Akshara</t>
+    <t>Admin</t>
   </si>
   <si>
-    <t>Swara</t>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -348,21 +354,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
addedd input.xlx with invalid credentials
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B88 Selenium\Workspace\framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E481B1B-3118-4C1B-AF9C-B1D753ED5F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AD1325C-BDC5-4569-81D7-3FC82E2F60F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Admin</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -356,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,4 +388,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530E7264-604C-410D-B8A9-341A8D989661}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>